<commit_message>
Testpiemēru pabeigšana, vēl tik testēšanas žurnāls
</commit_message>
<xml_diff>
--- a/LVT_Eksamens_TP_V_1_0_1.xlsx
+++ b/LVT_Eksamens_TP_V_1_0_1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="28695" windowHeight="12540" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="28695" windowHeight="12540" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Apraksts" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="227">
   <si>
     <t>Identifikatoru atšifrējums:</t>
   </si>
@@ -284,9 +284,6 @@
   </si>
   <si>
     <t xml:space="preserve">Jābūt startētai programmai </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Darbināt informācijas funkciju Main daļā </t>
   </si>
   <si>
     <t>1) Konsolē ievadīt atbilstošo ciparu "1"</t>
@@ -311,9 +308,6 @@
     <t>TP.MN.IN.02</t>
   </si>
   <si>
-    <t xml:space="preserve">Darbināt testa funkciju Main daļā </t>
-  </si>
-  <si>
     <t>1) Konsolē ievadīt atbilstošo ciparu "2"</t>
   </si>
   <si>
@@ -341,16 +335,10 @@
     <t>Lietotāja konsolē ievadīts "3"</t>
   </si>
   <si>
-    <t>Main daļā izvēles vietā ievadīt "x"</t>
-  </si>
-  <si>
     <t>1) Konsolē ievadīt atbilstošo simbolu "x"</t>
   </si>
   <si>
     <t>Lietotāja konsolē ievadīts "x"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Darbināt rezultāta parādīšanas funkciju Main daļā </t>
   </si>
   <si>
     <t>1) Tiks palaista funkcija
@@ -358,6 +346,374 @@
   </si>
   <si>
     <t>Jautājumu izvade</t>
+  </si>
+  <si>
+    <t>IZV</t>
+  </si>
+  <si>
+    <t>Izvade</t>
+  </si>
+  <si>
+    <t>IEV</t>
+  </si>
+  <si>
+    <t>Ievade</t>
+  </si>
+  <si>
+    <t>TP.IN.IEV.01</t>
+  </si>
+  <si>
+    <t>Jābūt palaistai informācijas funkcijai Main daļā</t>
+  </si>
+  <si>
+    <t>Izvada konsolē informāciju par testu</t>
+  </si>
+  <si>
+    <t>1) Tiks izvadīta informācija par testu
+2) Informācijas teksts būs ierāmēts četrstūri ASCII koda veidā</t>
+  </si>
+  <si>
+    <t>TP.TST.IEV.01</t>
+  </si>
+  <si>
+    <t>Jābūt palaistai testa funkcijai main daļā un jānodrošinas ka testa jautājums parādas</t>
+  </si>
+  <si>
+    <t>Pēc jautājuma atbilstoši pareizi ievadīt atbildi</t>
+  </si>
+  <si>
+    <t>1) Main daļā jāpalaiž testa funkcija
+2) Nodrošināt ka testa jautājums parādas
+3) Ievadīt atbilstoši pēc jautājuma atbildi, piemēram, 1 un 2 pareizi, tādēļ 12 vai 21</t>
+  </si>
+  <si>
+    <t>1) Main daļā jāpalaiž informācijas funkcija  konsolē ievadot "1"</t>
+  </si>
+  <si>
+    <t>Lietotāja konsolē atbilstoši jautājumam ievadīt atbildi</t>
+  </si>
+  <si>
+    <t>1) Tiks konsolē izvadīts "Pareizi"</t>
+  </si>
+  <si>
+    <t>TP.TST.IEV.02</t>
+  </si>
+  <si>
+    <t>Nepareizās atbildes ievade</t>
+  </si>
+  <si>
+    <t>Pēc jautājuma paradīšanās konsolē ievadīt nepareizu atbildi</t>
+  </si>
+  <si>
+    <t>1) Main daļā jāpalaiž testa funkcija
+2) Nodrošināt ka testa jautājums parādas
+3) Ievadīt nepareizu atbildi diapazona no 11 līdz 44</t>
+  </si>
+  <si>
+    <t>Lietotāja konsolē ievadīt nepareizu atbildi</t>
+  </si>
+  <si>
+    <t>1) Tiks konsolē izvadīts "Nepareizi"</t>
+  </si>
+  <si>
+    <t>TP.TST.REZ.OF.01</t>
+  </si>
+  <si>
+    <t>Jābūt palaistai testa funkcijai un uz visiem 10 testa jautājumiem atbildēt</t>
+  </si>
+  <si>
+    <t>Pēc testa pabeigšanas failā ierakstās rezultāts, cik pareizi, cik nepareizi</t>
+  </si>
+  <si>
+    <t>1) Main daļā jāpalaiž testa funkcija
+2) Atbildēt uz visiem 10 jautājumiem
+3) Atvērt failu "Rezultāti.txt" iekšā programmas atrašanās vietas mapē</t>
+  </si>
+  <si>
+    <t>Atvērt failu "Rezultāti.txt" iekšā programmas atrašanās vietas mapē</t>
+  </si>
+  <si>
+    <t>Tiks failā ierakstīts jaunā rindā tavs rezultāts, cik pareizi, cik nepareizi</t>
+  </si>
+  <si>
+    <t>TP.REZ.IZV.01</t>
+  </si>
+  <si>
+    <t>Jābūt palaistai rezultāta parādīšanas funkcijai</t>
+  </si>
+  <si>
+    <t>Palaidīsies rezultāta funkcija</t>
+  </si>
+  <si>
+    <t>Palaidīsies testa funkcija</t>
+  </si>
+  <si>
+    <t>Palaidīsies informācijas funkcija</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Izvadīsies konsolē rezultāta vēsture, cik iepriekš bijis pareizi, cik nepareizi </t>
+  </si>
+  <si>
+    <t>1) Main daļā jāpalaiž rezultāta parādīšanās funkcija  konsolē ievadot "3"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiks izvadīta rezultāta vēsture konsolē, cik iepriekš bijis pareizi, cik nepareizi </t>
+  </si>
+  <si>
+    <t>TP.MN.AIZ.01</t>
+  </si>
+  <si>
+    <t>Jābūt atvērtam "Teksta datnes tests" kodam</t>
+  </si>
+  <si>
+    <t>1) Konsolē jāievada simbols "x"</t>
+  </si>
+  <si>
+    <t>FN</t>
+  </si>
+  <si>
+    <t>Funkcija</t>
+  </si>
+  <si>
+    <t>TP.IN.FN.01</t>
+  </si>
+  <si>
+    <t>Jabūt ievadītam ciparam "1" konsolē</t>
+  </si>
+  <si>
+    <t>1) Konsolē jāievada cipars "1"</t>
+  </si>
+  <si>
+    <t>TP.IN.FN.02</t>
+  </si>
+  <si>
+    <t>Jabūt ievadītam ciparam "5" konsolē</t>
+  </si>
+  <si>
+    <t>Nepalaidīsies informācijas funkcija</t>
+  </si>
+  <si>
+    <t>Nepalaidīsies testa funkcija</t>
+  </si>
+  <si>
+    <t>Nepalaidīsies rezultāta funkcija</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nesāks darboties informācijas funkcija </t>
+  </si>
+  <si>
+    <t>1) Konsolē jāievada cipars "5"</t>
+  </si>
+  <si>
+    <t>1) Konsolē jāievada cipars "2"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sāks darboties mainTest funkcija </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sāks darboties infoTest funkcija </t>
+  </si>
+  <si>
+    <t>Jabūt ievadītam ciparam "2" konsolē</t>
+  </si>
+  <si>
+    <t>infoTest funkcijas darbināšana</t>
+  </si>
+  <si>
+    <t>mainTest funkcijas darbināšana</t>
+  </si>
+  <si>
+    <t>TP.TST.FN.01</t>
+  </si>
+  <si>
+    <t>TP.TST.FN.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nesāks darboties mainTest funkcija </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nesāks darboties results funkcija </t>
+  </si>
+  <si>
+    <t>results funkcijas darbināšana</t>
+  </si>
+  <si>
+    <t>Programma konsolē izvadīs "Nav tādas opcijas" un cikls ies no jauna</t>
+  </si>
+  <si>
+    <t>Programma palaidīts funkciju mainTest() un pēc funkcijas palaišanas cikls ies no jauna</t>
+  </si>
+  <si>
+    <t>Programma palaidīts funkciju infoTest() un pēc funkcijas palaišanas cikls ies no jauna</t>
+  </si>
+  <si>
+    <t>TP.REZ.FN.02</t>
+  </si>
+  <si>
+    <t>Jabūt ievadītam ciparam "3" konsolē</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sāks darboties results funkcija </t>
+  </si>
+  <si>
+    <t>1) Konsolē jāievada cipars "3"</t>
+  </si>
+  <si>
+    <t>Programma palaidīts funkciju results() un pēc funkcijas palaišanas cikls ies no jauna</t>
+  </si>
+  <si>
+    <t>TP.IN.FN.IZV.01</t>
+  </si>
+  <si>
+    <t>TP.Q.IEV.01</t>
+  </si>
+  <si>
+    <t>TP.Q.SC.01</t>
+  </si>
+  <si>
+    <t>TP.Q.IZV.01</t>
+  </si>
+  <si>
+    <t>PB</t>
+  </si>
+  <si>
+    <t>Pārbaude</t>
+  </si>
+  <si>
+    <t>TP.AT.PB.01</t>
+  </si>
+  <si>
+    <t>TP.AT.PB.02</t>
+  </si>
+  <si>
+    <t>TP.REZ.IF.IZV.01</t>
+  </si>
+  <si>
+    <t>TP.REZ.OF.IZV.01</t>
+  </si>
+  <si>
+    <t>Jābūt palaistai infoTest() funkcijai</t>
+  </si>
+  <si>
+    <t>Izvadīs konsolē informāciju par testu</t>
+  </si>
+  <si>
+    <t>1) Jāpalaīž funkcija infoTest()</t>
+  </si>
+  <si>
+    <t>Jāpalaīž funkcija infoTest()</t>
+  </si>
+  <si>
+    <t>Konsolē izvadīsies informācija par testu un Main() cikls sāksies no jauna</t>
+  </si>
+  <si>
+    <t>Jābūt palaistai mainTest() funkcijai</t>
+  </si>
+  <si>
+    <t>Masīvā questions saglabās 10 jautājumus</t>
+  </si>
+  <si>
+    <t>1) Jāpalaīž funkcija mainTest()</t>
+  </si>
+  <si>
+    <t>Jāpalaīž funkcija mainTest()</t>
+  </si>
+  <si>
+    <t>mainTest() funkcija palaidīs tālāk ciku funkciju randoms(), kas saglabās masīvā asked 10 nedublētus  (1-10) ciparus, kurus izmantos testa jautājumu kārtībai</t>
+  </si>
+  <si>
+    <t>Masīvā questions saglabāsies 10 jautājumi</t>
+  </si>
+  <si>
+    <t>Masīvā questions saglabāsies 10 nedublēti cipari</t>
+  </si>
+  <si>
+    <t>Pēc jautājumu ievadīšanas un jautājumu kārtības algoritma palaišanas pēc secības izvadīsies 10 jautājumi uz kuriem pieprasīta atbilde</t>
+  </si>
+  <si>
+    <t>Izvadīsies jautājums, pēc atbildes izvadīsies nakošais jautājums (visi jautājumi izvadās pēc secības algoritma)</t>
+  </si>
+  <si>
+    <t>Pareizas atbildes pārbaude atbilstošam jautājumam</t>
+  </si>
+  <si>
+    <t>1) Jāpalaīž funkcija mainTest()
+2) Jāievada pareiza atbilde atbilstošam jautājumam "Tava atbilde: " vietā</t>
+  </si>
+  <si>
+    <t>Pēc pareizas atbildes ievadīšanas ar if() pārbaudīs vai atbilde pareiza,piemēram, atbilde 1 vai 2, cikls pārbauda vai atbilde ir 12 vai 21, tad konsolē izvadās "Pareizi"</t>
+  </si>
+  <si>
+    <t>Jābūt palaistai mainTest() funkcijai un jāgaida līdz izvadas konsolē "Tava atbilde: ", tad jāievada nepareiza atbilde</t>
+  </si>
+  <si>
+    <t>Jābūt palaistai mainTest() funkcijai un jāgaida līdz izvadas konsolē "Tava atbilde: ", tad jāievada pareiza atbilde</t>
+  </si>
+  <si>
+    <t>Nepareizas atbildes pārbaude atbilstošam jautājumam</t>
+  </si>
+  <si>
+    <t>1) Jāpalaīž funkcija mainTest()
+2) Jāievada nepareiza atbilde atbilstošam jautājumam "Tava atbilde: " vietā</t>
+  </si>
+  <si>
+    <t>Konsolē ievadītai pareizai atbildei, kas atbilstošs jautājumam</t>
+  </si>
+  <si>
+    <t>Konsolē ievadītai nepareizai atbildei</t>
+  </si>
+  <si>
+    <t>1)Nepareizi ievadīt atbildi
+2) if() pārbaudīs vai atbilde pareiza,piemēram, atbilde 1 vai 2, cikls pārbauda vai atbilde ir 12 vai 21, bet tā kā nepareizi, cikls beigsies un izvadīsies "Nepareizi"</t>
+  </si>
+  <si>
+    <t>Jābūt palaistai mainTest() funkcijai un jāatbild uz visiem 10 jautājumiem</t>
+  </si>
+  <si>
+    <t>Lietotāja rezultātu ierakstīs failā jaunā rindā "rezultati.txt" un to pašu konsolē</t>
+  </si>
+  <si>
+    <t>1) Jāpalaīž funkcija mainTest()
+2) Jāatbild uz visiem 10 jautājumiem</t>
+  </si>
+  <si>
+    <t>Jāatbild uz visiem 10 jautājumiem</t>
+  </si>
+  <si>
+    <t>1) Rezultāts tiks ierakstīts ar ofstream palīdzību, cik pareizi, cik nepareizi
+2) Kā arī konsolē tiks izrakstīts cik pareizi, cik nepareizi</t>
+  </si>
+  <si>
+    <t>Jābūt palaistai results() funkcijai un jāatbild vismaz vienu reizi uz visiem 10 jautājumiem</t>
+  </si>
+  <si>
+    <t>Konsolē izvadīs rezultāta vēsturi, cik pareizi, cik nepareizi no faila "rezultati.txt"</t>
+  </si>
+  <si>
+    <t>1) Jāpalaīž funkcija mainTest()
+2) Jāatbild uz visiem 10 jautājumiem
+3) Jāpalaīž funkcija results()</t>
+  </si>
+  <si>
+    <t>Jāpalaīž funkcija results()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiks nolasīta ar ifstream palīdzību un izvadīta konsolē rezultāta vēsture </t>
+  </si>
+  <si>
+    <t>Bez faila "rezultati.txt" izveidošanās results() funkcijas palaišana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jābūt palaistai results() funkcijai, bez iepriekš pildīta testa vai faila "rezultati.txt" izdzēšanas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jāpalaīž funkcija results() un iepriekš nepildīta testa vai faila "rezultati.txt" izdzēšanas </t>
+  </si>
+  <si>
+    <t>ifstream neatrod failu un results() beidzas, Main() cikls atsāk no jauna</t>
+  </si>
+  <si>
+    <t>Cikls beigsies, konsolē parādīsies "Programma beidzas!" un programma izslēgsies, pieeja pie konsoles pazudīs</t>
   </si>
 </sst>
 </file>
@@ -503,7 +859,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -548,6 +904,22 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -571,26 +943,11 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -890,18 +1247,18 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4" ht="20.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1"/>
@@ -910,20 +1267,20 @@
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1"/>
@@ -952,12 +1309,12 @@
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
@@ -1070,26 +1427,42 @@
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="2"/>
-      <c r="B20" s="3"/>
+      <c r="A20" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>110</v>
+      </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="4"/>
-      <c r="B21" s="1"/>
+      <c r="A21" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>112</v>
+      </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="4"/>
-      <c r="B22" s="1"/>
+      <c r="A22" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>148</v>
+      </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="4"/>
-      <c r="B23" s="1"/>
+      <c r="A23" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>183</v>
+      </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
@@ -1114,8 +1487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1133,8 +1506,8 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="30"/>
-      <c r="B2" s="29"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="35"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="6" t="s">
@@ -1145,10 +1518,10 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="29"/>
+      <c r="B4" s="35"/>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="6" t="s">
@@ -1179,14 +1552,14 @@
         <v>35</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="29"/>
+      <c r="B9" s="35"/>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="6" t="s">
@@ -1197,10 +1570,10 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="29"/>
+      <c r="B11" s="35"/>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="6" t="s">
@@ -1223,7 +1596,7 @@
         <v>38</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1251,10 +1624,10 @@
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="29"/>
+      <c r="B18" s="35"/>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="6" t="s">
@@ -1265,8 +1638,8 @@
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="30"/>
-      <c r="B20" s="29"/>
+      <c r="A20" s="36"/>
+      <c r="B20" s="35"/>
     </row>
     <row r="21" spans="1:2" ht="37.5" customHeight="1">
       <c r="A21" s="8"/>
@@ -1292,16 +1665,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H99"/>
+  <dimension ref="A1:H100"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62:H62"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K58" sqref="K58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="7" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" customWidth="1"/>
+    <col min="4" max="7" width="25.7109375" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1332,16 +1708,16 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
     </row>
     <row r="3" spans="1:8" ht="60">
       <c r="A3" s="6" t="s">
@@ -1370,16 +1746,16 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="32"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-    </row>
-    <row r="5" spans="1:8" ht="45">
+      <c r="A4" s="38"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+    </row>
+    <row r="5" spans="1:8" ht="60">
       <c r="A5" s="6" t="s">
         <v>80</v>
       </c>
@@ -1387,16 +1763,16 @@
         <v>81</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>107</v>
+        <v>72</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E5" s="37" t="s">
-        <v>108</v>
-      </c>
-      <c r="F5" s="37" t="s">
-        <v>109</v>
+      <c r="E5" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>106</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>85</v>
@@ -1406,350 +1782,420 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="32"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
+      <c r="A6" s="38"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
     </row>
     <row r="7" spans="1:8" ht="45">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="D7" s="37" t="s">
+      <c r="D7" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="E7" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="E7" s="37" t="s">
+      <c r="F7" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="F7" s="37" t="s">
+      <c r="G7" s="27" t="s">
         <v>91</v>
-      </c>
-      <c r="G7" s="37" t="s">
-        <v>92</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="45">
-      <c r="A8" s="36" t="s">
-        <v>96</v>
-      </c>
-      <c r="B8" s="37" t="s">
+      <c r="A8" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="D8" s="37" t="s">
-        <v>89</v>
-      </c>
-      <c r="E8" s="37" t="s">
+      <c r="D8" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="F8" s="37" t="s">
+      <c r="G8" s="28" t="s">
         <v>94</v>
-      </c>
-      <c r="G8" s="38" t="s">
-        <v>95</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="32"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
+      <c r="A9" s="38"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
     </row>
     <row r="10" spans="1:8" ht="60">
-      <c r="A10" s="36" t="s">
-        <v>100</v>
-      </c>
-      <c r="B10" s="37" t="s">
+      <c r="A10" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="D10" s="37" t="s">
+      <c r="D10" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="F10" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="E10" s="37" t="s">
-        <v>98</v>
-      </c>
-      <c r="F10" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="G10" s="37" t="s">
-        <v>111</v>
+      <c r="G10" s="27" t="s">
+        <v>107</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="45">
-      <c r="A11" s="36" t="s">
-        <v>101</v>
-      </c>
-      <c r="B11" s="37" t="s">
+      <c r="A11" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="D11" s="37" t="s">
-        <v>97</v>
-      </c>
-      <c r="E11" s="37" t="s">
+      <c r="D11" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="F11" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="F11" s="37" t="s">
+      <c r="G11" s="28" t="s">
         <v>94</v>
-      </c>
-      <c r="G11" s="38" t="s">
-        <v>95</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="32"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
+      <c r="A12" s="38"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
     </row>
     <row r="13" spans="1:8" ht="45">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="C13" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="F13" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="C13" s="37" t="s">
-        <v>88</v>
-      </c>
-      <c r="D13" s="37" t="s">
-        <v>110</v>
-      </c>
-      <c r="E13" s="37" t="s">
-        <v>105</v>
-      </c>
-      <c r="F13" s="37" t="s">
-        <v>106</v>
-      </c>
-      <c r="G13" s="37" t="s">
-        <v>92</v>
+      <c r="G13" s="27" t="s">
+        <v>91</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="45">
-      <c r="A14" s="36" t="s">
-        <v>103</v>
+      <c r="A14" s="26" t="s">
+        <v>101</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="C14" s="37" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="D14" s="37" t="s">
-        <v>97</v>
-      </c>
-      <c r="E14" s="37" t="s">
+      <c r="D14" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="F14" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="F14" s="37" t="s">
+      <c r="G14" s="28" t="s">
         <v>94</v>
-      </c>
-      <c r="G14" s="38" t="s">
-        <v>95</v>
       </c>
       <c r="H14" s="7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="32"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="6" t="s">
+      <c r="A15" s="38"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+    </row>
+    <row r="16" spans="1:8" ht="75">
+      <c r="A16" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F16" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="H16" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="32"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="6" t="s">
+      <c r="A17" s="38"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+    </row>
+    <row r="18" spans="1:8" ht="120">
+      <c r="A18" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="H18" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="6" t="s">
+    <row r="19" spans="1:8" ht="90">
+      <c r="A19" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="H19" s="7" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="32"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="6" t="s">
+      <c r="A20" s="38"/>
+      <c r="B20" s="39"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="39"/>
+    </row>
+    <row r="21" spans="1:8" ht="105">
+      <c r="A21" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="H21" s="7" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="32"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="6" t="s">
+      <c r="A22" s="38"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
+    </row>
+    <row r="23" spans="1:8" ht="45">
+      <c r="A23" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="F23" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="H23" s="7" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="32"/>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="34"/>
+      <c r="A24" s="38"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="39"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="39"/>
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="37"/>
-      <c r="H25" s="39"/>
+      <c r="A25" s="29"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="29"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="35"/>
-      <c r="B26" s="37"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="37"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="39"/>
-      <c r="B27" s="39"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="39"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="39"/>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
+      <c r="A28" s="29"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="35"/>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
+      <c r="A29" s="25"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="7"/>
@@ -1772,356 +2218,582 @@
       <c r="H31" s="7"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="32" t="s">
+      <c r="A32" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="34"/>
-      <c r="H32" s="34"/>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="6" t="s">
+      <c r="B32" s="39"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="39"/>
+    </row>
+    <row r="33" spans="1:8" ht="75">
+      <c r="A33" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F33" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="H33" s="7" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="32"/>
-      <c r="B34" s="34"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="34"/>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="6" t="s">
+      <c r="A34" s="38"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="38"/>
+    </row>
+    <row r="35" spans="1:8" ht="60">
+      <c r="A35" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="B35" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="F35" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="H35" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="6" t="s">
+    <row r="36" spans="1:8" ht="45">
+      <c r="A36" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B36" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="F36" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="H36" s="7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="32"/>
-      <c r="B37" s="34"/>
-      <c r="C37" s="34"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
-      <c r="G37" s="34"/>
-      <c r="H37" s="34"/>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="6" t="s">
+      <c r="A37" s="38"/>
+      <c r="B37" s="39"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="39"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="39"/>
+      <c r="H37" s="39"/>
+    </row>
+    <row r="38" spans="1:8" ht="60">
+      <c r="A38" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="B38" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="F38" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="H38" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="6" t="s">
+    <row r="39" spans="1:8" ht="45">
+      <c r="A39" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B39" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="F39" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="H39" s="7" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="32"/>
-      <c r="B40" s="34"/>
-      <c r="C40" s="34"/>
-      <c r="D40" s="34"/>
-      <c r="E40" s="34"/>
-      <c r="F40" s="34"/>
-      <c r="G40" s="34"/>
-      <c r="H40" s="34"/>
-    </row>
-    <row r="41" spans="1:8">
-      <c r="A41" s="7"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="6" t="s">
+      <c r="A40" s="38"/>
+      <c r="B40" s="39"/>
+      <c r="C40" s="39"/>
+      <c r="D40" s="39"/>
+      <c r="E40" s="39"/>
+      <c r="F40" s="39"/>
+      <c r="G40" s="39"/>
+      <c r="H40" s="39"/>
+    </row>
+    <row r="41" spans="1:8" ht="60">
+      <c r="A41" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="B41" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="F41" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="H41" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
-      <c r="A42" s="7"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="6" t="s">
+    <row r="42" spans="1:8" ht="45">
+      <c r="A42" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="B42" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="F42" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="H42" s="7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="32"/>
-      <c r="B43" s="34"/>
-      <c r="C43" s="34"/>
-      <c r="D43" s="34"/>
-      <c r="E43" s="34"/>
-      <c r="F43" s="34"/>
-      <c r="G43" s="34"/>
-      <c r="H43" s="34"/>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="A44" s="7"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="6" t="s">
+      <c r="A43" s="38"/>
+      <c r="B43" s="39"/>
+      <c r="C43" s="39"/>
+      <c r="D43" s="39"/>
+      <c r="E43" s="39"/>
+      <c r="F43" s="39"/>
+      <c r="G43" s="39"/>
+      <c r="H43" s="39"/>
+    </row>
+    <row r="44" spans="1:8" ht="60">
+      <c r="A44" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="H44" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="32"/>
-      <c r="B45" s="34"/>
-      <c r="C45" s="34"/>
-      <c r="D45" s="34"/>
-      <c r="E45" s="34"/>
-      <c r="F45" s="34"/>
-      <c r="G45" s="34"/>
-      <c r="H45" s="34"/>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="A46" s="7"/>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="6" t="s">
+      <c r="A45" s="38"/>
+      <c r="B45" s="39"/>
+      <c r="C45" s="39"/>
+      <c r="D45" s="39"/>
+      <c r="E45" s="39"/>
+      <c r="F45" s="39"/>
+      <c r="G45" s="39"/>
+      <c r="H45" s="39"/>
+    </row>
+    <row r="46" spans="1:8" ht="30">
+      <c r="A46" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="H46" s="7" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="32"/>
-      <c r="B47" s="34"/>
-      <c r="C47" s="34"/>
-      <c r="D47" s="34"/>
-      <c r="E47" s="34"/>
-      <c r="F47" s="34"/>
-      <c r="G47" s="34"/>
-      <c r="H47" s="34"/>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="12"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7"/>
-      <c r="G48" s="7"/>
-      <c r="H48" s="6" t="s">
+      <c r="A47" s="38"/>
+      <c r="B47" s="39"/>
+      <c r="C47" s="39"/>
+      <c r="D47" s="39"/>
+      <c r="E47" s="39"/>
+      <c r="F47" s="39"/>
+      <c r="G47" s="39"/>
+      <c r="H47" s="39"/>
+    </row>
+    <row r="48" spans="1:8" ht="105">
+      <c r="A48" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="H48" s="7" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="32"/>
-      <c r="B49" s="34"/>
-      <c r="C49" s="34"/>
-      <c r="D49" s="34"/>
-      <c r="E49" s="34"/>
-      <c r="F49" s="34"/>
-      <c r="G49" s="34"/>
-      <c r="H49" s="34"/>
-    </row>
-    <row r="50" spans="1:8">
-      <c r="A50" s="12"/>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
-      <c r="G50" s="7"/>
-      <c r="H50" s="6" t="s">
+      <c r="A49" s="38"/>
+      <c r="B49" s="39"/>
+      <c r="C49" s="39"/>
+      <c r="D49" s="39"/>
+      <c r="E49" s="39"/>
+      <c r="F49" s="39"/>
+      <c r="G49" s="39"/>
+      <c r="H49" s="39"/>
+    </row>
+    <row r="50" spans="1:8" ht="90">
+      <c r="A50" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="G50" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="H50" s="7" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="32"/>
-      <c r="B51" s="34"/>
-      <c r="C51" s="34"/>
-      <c r="D51" s="34"/>
-      <c r="E51" s="34"/>
-      <c r="F51" s="34"/>
-      <c r="G51" s="34"/>
-      <c r="H51" s="34"/>
-    </row>
-    <row r="52" spans="1:8">
-      <c r="A52" s="12"/>
-      <c r="B52" s="7"/>
-      <c r="C52" s="7"/>
-      <c r="D52" s="7"/>
-      <c r="E52" s="7"/>
-      <c r="F52" s="7"/>
-      <c r="G52" s="7"/>
-      <c r="H52" s="6" t="s">
+      <c r="A51" s="38"/>
+      <c r="B51" s="39"/>
+      <c r="C51" s="39"/>
+      <c r="D51" s="39"/>
+      <c r="E51" s="39"/>
+      <c r="F51" s="39"/>
+      <c r="G51" s="39"/>
+      <c r="H51" s="39"/>
+    </row>
+    <row r="52" spans="1:8" ht="105">
+      <c r="A52" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="H52" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
-      <c r="A53" s="12"/>
-      <c r="B53" s="7"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="7"/>
-      <c r="G53" s="7"/>
-      <c r="H53" s="6" t="s">
+    <row r="53" spans="1:8" ht="105">
+      <c r="A53" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="H53" s="7" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="32"/>
-      <c r="B54" s="34"/>
-      <c r="C54" s="34"/>
-      <c r="D54" s="34"/>
-      <c r="E54" s="34"/>
-      <c r="F54" s="34"/>
-      <c r="G54" s="34"/>
-      <c r="H54" s="34"/>
-    </row>
-    <row r="55" spans="1:8">
-      <c r="A55" s="7"/>
-      <c r="B55" s="7"/>
-      <c r="C55" s="7"/>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="7"/>
-      <c r="G55" s="7"/>
-      <c r="H55" s="6" t="s">
+      <c r="A54" s="38"/>
+      <c r="B54" s="39"/>
+      <c r="C54" s="39"/>
+      <c r="D54" s="39"/>
+      <c r="E54" s="39"/>
+      <c r="F54" s="39"/>
+      <c r="G54" s="39"/>
+      <c r="H54" s="39"/>
+    </row>
+    <row r="55" spans="1:8" ht="90">
+      <c r="A55" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="H55" s="7" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="32"/>
-      <c r="B56" s="34"/>
-      <c r="C56" s="34"/>
-      <c r="D56" s="34"/>
-      <c r="E56" s="34"/>
-      <c r="F56" s="34"/>
-      <c r="G56" s="34"/>
-      <c r="H56" s="34"/>
-    </row>
-    <row r="57" spans="1:8">
-      <c r="A57" s="7"/>
-      <c r="B57" s="7"/>
-      <c r="C57" s="7"/>
-      <c r="D57" s="7"/>
-      <c r="E57" s="7"/>
-      <c r="F57" s="7"/>
-      <c r="G57" s="7"/>
-      <c r="H57" s="6" t="s">
+      <c r="A56" s="38"/>
+      <c r="B56" s="39"/>
+      <c r="C56" s="39"/>
+      <c r="D56" s="39"/>
+      <c r="E56" s="39"/>
+      <c r="F56" s="39"/>
+      <c r="G56" s="39"/>
+      <c r="H56" s="39"/>
+    </row>
+    <row r="57" spans="1:8" ht="75">
+      <c r="A57" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="G57" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="H57" s="7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
-      <c r="A58" s="39"/>
-      <c r="B58" s="39"/>
-      <c r="C58" s="39"/>
-      <c r="D58" s="39"/>
-      <c r="E58" s="39"/>
-      <c r="F58" s="39"/>
-      <c r="G58" s="39"/>
-      <c r="H58" s="39"/>
+    <row r="58" spans="1:8" ht="60">
+      <c r="A58" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="G58" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="H58" s="7" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="59" spans="1:8">
-      <c r="A59" s="35"/>
-      <c r="B59" s="37"/>
-      <c r="C59" s="37"/>
-      <c r="D59" s="37"/>
-      <c r="E59" s="37"/>
-      <c r="F59" s="37"/>
-      <c r="G59" s="37"/>
-      <c r="H59" s="37"/>
+      <c r="A59" s="38"/>
+      <c r="B59" s="39"/>
+      <c r="C59" s="39"/>
+      <c r="D59" s="39"/>
+      <c r="E59" s="39"/>
+      <c r="F59" s="39"/>
+      <c r="G59" s="39"/>
+      <c r="H59" s="39"/>
     </row>
     <row r="60" spans="1:8">
-      <c r="A60" s="39"/>
-      <c r="B60" s="39"/>
-      <c r="C60" s="39"/>
-      <c r="D60" s="39"/>
-      <c r="E60" s="39"/>
-      <c r="F60" s="39"/>
-      <c r="G60" s="39"/>
-      <c r="H60" s="39"/>
+      <c r="A60" s="25"/>
+      <c r="B60" s="27"/>
+      <c r="C60" s="27"/>
+      <c r="D60" s="27"/>
+      <c r="E60" s="27"/>
+      <c r="F60" s="27"/>
+      <c r="G60" s="27"/>
+      <c r="H60" s="27"/>
     </row>
     <row r="61" spans="1:8">
-      <c r="A61" s="39"/>
-      <c r="B61" s="39"/>
-      <c r="C61" s="39"/>
-      <c r="D61" s="39"/>
-      <c r="E61" s="39"/>
-      <c r="F61" s="39"/>
-      <c r="G61" s="39"/>
-      <c r="H61" s="39"/>
+      <c r="A61" s="29"/>
+      <c r="B61" s="29"/>
+      <c r="C61" s="29"/>
+      <c r="D61" s="29"/>
+      <c r="E61" s="29"/>
+      <c r="F61" s="29"/>
+      <c r="G61" s="29"/>
+      <c r="H61" s="29"/>
     </row>
     <row r="62" spans="1:8">
-      <c r="A62" s="35"/>
-      <c r="B62" s="37"/>
-      <c r="C62" s="37"/>
-      <c r="D62" s="37"/>
-      <c r="E62" s="37"/>
-      <c r="F62" s="37"/>
-      <c r="G62" s="37"/>
-      <c r="H62" s="37"/>
+      <c r="A62" s="29"/>
+      <c r="B62" s="29"/>
+      <c r="C62" s="29"/>
+      <c r="D62" s="29"/>
+      <c r="E62" s="29"/>
+      <c r="F62" s="29"/>
+      <c r="G62" s="29"/>
+      <c r="H62" s="29"/>
     </row>
     <row r="63" spans="1:8">
-      <c r="A63" s="7"/>
-      <c r="B63" s="7"/>
-      <c r="C63" s="7"/>
-      <c r="D63" s="7"/>
-      <c r="E63" s="7"/>
-      <c r="F63" s="7"/>
-      <c r="G63" s="7"/>
-      <c r="H63" s="7"/>
+      <c r="A63" s="25"/>
+      <c r="B63" s="27"/>
+      <c r="C63" s="27"/>
+      <c r="D63" s="27"/>
+      <c r="E63" s="27"/>
+      <c r="F63" s="27"/>
+      <c r="G63" s="27"/>
+      <c r="H63" s="27"/>
     </row>
     <row r="64" spans="1:8">
       <c r="A64" s="7"/>
@@ -2177,64 +2849,64 @@
       <c r="A69" s="7"/>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
+      <c r="D69" s="7"/>
+      <c r="E69" s="7"/>
+      <c r="F69" s="7"/>
+      <c r="G69" s="7"/>
       <c r="H69" s="7"/>
     </row>
     <row r="70" spans="1:8">
-      <c r="A70" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
+      <c r="A70" s="7"/>
+      <c r="B70" s="7"/>
+      <c r="C70" s="7"/>
       <c r="D70" s="1"/>
-      <c r="E70" s="13" t="s">
-        <v>52</v>
-      </c>
+      <c r="E70" s="1"/>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
       <c r="H70" s="7"/>
     </row>
-    <row r="71" spans="1:8" ht="25.5">
-      <c r="A71" s="14" t="s">
+    <row r="71" spans="1:8">
+      <c r="A71" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="7"/>
+    </row>
+    <row r="72" spans="1:8" ht="25.5">
+      <c r="A72" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="B71" s="14" t="s">
+      <c r="B72" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C71" s="14" t="s">
+      <c r="C72" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D71" s="1"/>
-      <c r="E71" s="14" t="s">
+      <c r="D72" s="1"/>
+      <c r="E72" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="F71" s="14" t="s">
+      <c r="F72" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G71" s="14" t="s">
+      <c r="G72" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="H71" s="7"/>
-    </row>
-    <row r="72" spans="1:8">
-      <c r="A72" s="6"/>
-      <c r="B72" s="6"/>
-      <c r="C72" s="15"/>
-      <c r="D72" s="1"/>
-      <c r="E72" s="6"/>
-      <c r="F72" s="6"/>
-      <c r="G72" s="15"/>
       <c r="H72" s="7"/>
     </row>
     <row r="73" spans="1:8">
-      <c r="A73" s="1"/>
+      <c r="A73" s="6"/>
       <c r="B73" s="6"/>
       <c r="C73" s="15"/>
       <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
+      <c r="E73" s="6"/>
       <c r="F73" s="6"/>
       <c r="G73" s="15"/>
       <c r="H73" s="7"/>
@@ -2245,160 +2917,160 @@
       <c r="C74" s="15"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
-      <c r="F74" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="G74" s="17"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="15"/>
       <c r="H74" s="7"/>
     </row>
     <row r="75" spans="1:8">
       <c r="A75" s="1"/>
-      <c r="B75" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C75" s="17"/>
+      <c r="B75" s="6"/>
+      <c r="C75" s="15"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
-      <c r="G75" s="1"/>
+      <c r="F75" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G75" s="17"/>
       <c r="H75" s="7"/>
     </row>
     <row r="76" spans="1:8">
       <c r="A76" s="1"/>
-      <c r="B76" s="1"/>
-      <c r="C76" s="1"/>
+      <c r="B76" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C76" s="17"/>
       <c r="D76" s="1"/>
-      <c r="E76" s="33" t="s">
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="7"/>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="F76" s="25"/>
-      <c r="G76" s="25"/>
-      <c r="H76" s="7"/>
-    </row>
-    <row r="77" spans="1:8" ht="25.5">
-      <c r="A77" s="14" t="s">
+      <c r="F77" s="31"/>
+      <c r="G77" s="31"/>
+      <c r="H77" s="7"/>
+    </row>
+    <row r="78" spans="1:8" ht="25.5">
+      <c r="A78" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="B77" s="14" t="s">
+      <c r="B78" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C77" s="14" t="s">
+      <c r="C78" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D77" s="1"/>
-      <c r="E77" s="14" t="s">
+      <c r="D78" s="1"/>
+      <c r="E78" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="F77" s="14" t="s">
+      <c r="F78" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G77" s="14" t="s">
+      <c r="G78" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="H77" s="7"/>
-    </row>
-    <row r="78" spans="1:8">
-      <c r="A78" s="6"/>
-      <c r="B78" s="6"/>
-      <c r="C78" s="1"/>
-      <c r="D78" s="1"/>
-      <c r="E78" s="6"/>
-      <c r="F78" s="12"/>
-      <c r="G78" s="18"/>
       <c r="H78" s="7"/>
     </row>
     <row r="79" spans="1:8">
-      <c r="A79" s="1"/>
-      <c r="B79" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C79" s="17"/>
+      <c r="A79" s="6"/>
+      <c r="B79" s="6"/>
+      <c r="C79" s="1"/>
       <c r="D79" s="1"/>
-      <c r="E79" s="1"/>
+      <c r="E79" s="6"/>
       <c r="F79" s="12"/>
       <c r="G79" s="18"/>
       <c r="H79" s="7"/>
     </row>
     <row r="80" spans="1:8">
       <c r="A80" s="1"/>
-      <c r="B80" s="1"/>
-      <c r="C80" s="1"/>
+      <c r="B80" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C80" s="17"/>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
       <c r="F80" s="12"/>
       <c r="G80" s="18"/>
       <c r="H80" s="7"/>
     </row>
-    <row r="81" spans="1:8" ht="25.5">
-      <c r="A81" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B81" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C81" s="14" t="s">
-        <v>54</v>
-      </c>
+    <row r="81" spans="1:8">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
       <c r="F81" s="12"/>
       <c r="G81" s="18"/>
       <c r="H81" s="7"/>
     </row>
-    <row r="82" spans="1:8">
-      <c r="A82" s="6"/>
-      <c r="B82" s="6"/>
-      <c r="C82" s="1"/>
+    <row r="82" spans="1:8" ht="25.5">
+      <c r="A82" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B82" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C82" s="14" t="s">
+        <v>54</v>
+      </c>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
-      <c r="F82" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="G82" s="17"/>
+      <c r="F82" s="12"/>
+      <c r="G82" s="18"/>
       <c r="H82" s="7"/>
     </row>
     <row r="83" spans="1:8">
-      <c r="A83" s="1"/>
-      <c r="B83" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C83" s="17"/>
+      <c r="A83" s="6"/>
+      <c r="B83" s="6"/>
+      <c r="C83" s="1"/>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
-      <c r="F83" s="1"/>
-      <c r="G83" s="1"/>
+      <c r="F83" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G83" s="17"/>
       <c r="H83" s="7"/>
     </row>
     <row r="84" spans="1:8">
       <c r="A84" s="1"/>
-      <c r="B84" s="1"/>
-      <c r="C84" s="1"/>
+      <c r="B84" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C84" s="17"/>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
       <c r="H84" s="7"/>
     </row>
-    <row r="85" spans="1:8" ht="25.5">
-      <c r="A85" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B85" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C85" s="14" t="s">
-        <v>54</v>
-      </c>
+    <row r="85" spans="1:8">
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
+      <c r="C85" s="1"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
       <c r="H85" s="7"/>
     </row>
-    <row r="86" spans="1:8">
-      <c r="A86" s="6"/>
-      <c r="B86" s="6"/>
-      <c r="C86" s="1"/>
+    <row r="86" spans="1:8" ht="25.5">
+      <c r="A86" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B86" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C86" s="14" t="s">
+        <v>54</v>
+      </c>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
@@ -2406,11 +3078,9 @@
       <c r="H86" s="7"/>
     </row>
     <row r="87" spans="1:8">
-      <c r="A87" s="1"/>
-      <c r="B87" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C87" s="17"/>
+      <c r="A87" s="6"/>
+      <c r="B87" s="6"/>
+      <c r="C87" s="1"/>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
@@ -2419,8 +3089,10 @@
     </row>
     <row r="88" spans="1:8">
       <c r="A88" s="1"/>
-      <c r="B88" s="1"/>
-      <c r="C88" s="1"/>
+      <c r="B88" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C88" s="17"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
@@ -2437,26 +3109,26 @@
       <c r="G89" s="1"/>
       <c r="H89" s="7"/>
     </row>
-    <row r="90" spans="1:8" ht="25.5">
-      <c r="A90" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B90" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C90" s="14" t="s">
-        <v>54</v>
-      </c>
+    <row r="90" spans="1:8">
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
+      <c r="C90" s="1"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
-      <c r="H90" s="1"/>
-    </row>
-    <row r="91" spans="1:8">
-      <c r="A91" s="6"/>
-      <c r="B91" s="7"/>
-      <c r="C91" s="19"/>
+      <c r="H90" s="7"/>
+    </row>
+    <row r="91" spans="1:8" ht="25.5">
+      <c r="A91" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B91" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C91" s="14" t="s">
+        <v>54</v>
+      </c>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
@@ -2464,7 +3136,7 @@
       <c r="H91" s="1"/>
     </row>
     <row r="92" spans="1:8">
-      <c r="A92" s="1"/>
+      <c r="A92" s="6"/>
       <c r="B92" s="7"/>
       <c r="C92" s="19"/>
       <c r="D92" s="1"/>
@@ -2525,8 +3197,8 @@
     </row>
     <row r="98" spans="1:8">
       <c r="A98" s="1"/>
-      <c r="B98" s="1"/>
-      <c r="C98" s="1"/>
+      <c r="B98" s="7"/>
+      <c r="C98" s="19"/>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
@@ -2535,24 +3207,36 @@
     </row>
     <row r="99" spans="1:8">
       <c r="A99" s="1"/>
-      <c r="B99" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C99" s="17"/>
+      <c r="B99" s="1"/>
+      <c r="C99" s="1"/>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
       <c r="G99" s="1"/>
       <c r="H99" s="1"/>
     </row>
+    <row r="100" spans="1:8">
+      <c r="A100" s="1"/>
+      <c r="B100" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C100" s="17"/>
+      <c r="D100" s="1"/>
+      <c r="E100" s="1"/>
+      <c r="F100" s="1"/>
+      <c r="G100" s="1"/>
+      <c r="H100" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A12:H12"/>
+  <mergeCells count="23">
+    <mergeCell ref="E77:G77"/>
+    <mergeCell ref="A45:H45"/>
+    <mergeCell ref="A47:H47"/>
+    <mergeCell ref="A49:H49"/>
+    <mergeCell ref="A51:H51"/>
+    <mergeCell ref="A54:H54"/>
+    <mergeCell ref="A56:H56"/>
+    <mergeCell ref="A59:H59"/>
     <mergeCell ref="A43:H43"/>
     <mergeCell ref="A17:H17"/>
     <mergeCell ref="A20:H20"/>
@@ -2562,13 +3246,12 @@
     <mergeCell ref="A34:H34"/>
     <mergeCell ref="A37:H37"/>
     <mergeCell ref="A40:H40"/>
-    <mergeCell ref="E76:G76"/>
-    <mergeCell ref="A45:H45"/>
-    <mergeCell ref="A47:H47"/>
-    <mergeCell ref="A49:H49"/>
-    <mergeCell ref="A51:H51"/>
-    <mergeCell ref="A54:H54"/>
-    <mergeCell ref="A56:H56"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A12:H12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2579,8 +3262,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P29" sqref="P29"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -2627,16 +3311,16 @@
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -2655,14 +3339,14 @@
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="32"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
+      <c r="A4" s="38"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -2694,14 +3378,14 @@
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="32"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
+      <c r="A7" s="38"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -2733,14 +3417,14 @@
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="32"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
+      <c r="A10" s="38"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -2772,14 +3456,14 @@
       <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="32"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
+      <c r="A13" s="38"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -2798,14 +3482,14 @@
       <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1">
-      <c r="A15" s="32"/>
-      <c r="B15" s="32"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
+      <c r="A15" s="38"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -2824,14 +3508,14 @@
       <c r="K16" s="1"/>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1">
-      <c r="A17" s="32"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
+      <c r="A17" s="38"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -2863,14 +3547,14 @@
       <c r="K19" s="1"/>
     </row>
     <row r="20" spans="1:11" ht="15" customHeight="1">
-      <c r="A20" s="32"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="39"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="39"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -2902,14 +3586,14 @@
       <c r="K22" s="1"/>
     </row>
     <row r="23" spans="1:11" ht="15" customHeight="1">
-      <c r="A23" s="32"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
+      <c r="A23" s="38"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -2928,14 +3612,14 @@
       <c r="K24" s="1"/>
     </row>
     <row r="25" spans="1:11" ht="15" customHeight="1">
-      <c r="A25" s="32"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
+      <c r="A25" s="38"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="39"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
@@ -2954,14 +3638,14 @@
       <c r="K26" s="1"/>
     </row>
     <row r="27" spans="1:11" ht="15" customHeight="1">
-      <c r="A27" s="32"/>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
+      <c r="A27" s="38"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="39"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
@@ -2993,14 +3677,14 @@
       <c r="K29" s="1"/>
     </row>
     <row r="30" spans="1:11" ht="15" customHeight="1">
-      <c r="A30" s="32"/>
-      <c r="B30" s="34"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="34"/>
-      <c r="H30" s="34"/>
+      <c r="A30" s="38"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
@@ -3032,16 +3716,16 @@
       <c r="K32" s="1"/>
     </row>
     <row r="33" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A33" s="32" t="s">
+      <c r="A33" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="B33" s="29"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="29"/>
-      <c r="H33" s="29"/>
+      <c r="B33" s="35"/>
+      <c r="C33" s="35"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="35"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
@@ -3060,14 +3744,14 @@
       <c r="K34" s="1"/>
     </row>
     <row r="35" spans="1:11" ht="18" customHeight="1">
-      <c r="A35" s="32"/>
-      <c r="B35" s="29"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="29"/>
-      <c r="H35" s="29"/>
+      <c r="A35" s="38"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="35"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -3086,14 +3770,14 @@
       <c r="K36" s="1"/>
     </row>
     <row r="37" spans="1:11" ht="17.25" customHeight="1">
-      <c r="A37" s="32"/>
-      <c r="B37" s="29"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="29"/>
-      <c r="H37" s="29"/>
+      <c r="A37" s="38"/>
+      <c r="B37" s="35"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="35"/>
+      <c r="G37" s="35"/>
+      <c r="H37" s="35"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
@@ -3125,14 +3809,14 @@
       <c r="K39" s="1"/>
     </row>
     <row r="40" spans="1:11" ht="20.25" customHeight="1">
-      <c r="A40" s="32"/>
-      <c r="B40" s="29"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="29"/>
+      <c r="A40" s="38"/>
+      <c r="B40" s="35"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="35"/>
+      <c r="H40" s="35"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
@@ -3164,14 +3848,14 @@
       <c r="K42" s="1"/>
     </row>
     <row r="43" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A43" s="32"/>
-      <c r="B43" s="29"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29"/>
-      <c r="G43" s="29"/>
-      <c r="H43" s="29"/>
+      <c r="A43" s="38"/>
+      <c r="B43" s="35"/>
+      <c r="C43" s="35"/>
+      <c r="D43" s="35"/>
+      <c r="E43" s="35"/>
+      <c r="F43" s="35"/>
+      <c r="G43" s="35"/>
+      <c r="H43" s="35"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
@@ -3216,14 +3900,14 @@
       <c r="K46" s="1"/>
     </row>
     <row r="47" spans="1:11" ht="18" customHeight="1">
-      <c r="A47" s="32"/>
-      <c r="B47" s="29"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="29"/>
-      <c r="E47" s="29"/>
-      <c r="F47" s="29"/>
-      <c r="G47" s="29"/>
-      <c r="H47" s="29"/>
+      <c r="A47" s="38"/>
+      <c r="B47" s="35"/>
+      <c r="C47" s="35"/>
+      <c r="D47" s="35"/>
+      <c r="E47" s="35"/>
+      <c r="F47" s="35"/>
+      <c r="G47" s="35"/>
+      <c r="H47" s="35"/>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
@@ -3268,14 +3952,14 @@
       <c r="K50" s="1"/>
     </row>
     <row r="51" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A51" s="32"/>
-      <c r="B51" s="29"/>
-      <c r="C51" s="29"/>
-      <c r="D51" s="29"/>
-      <c r="E51" s="29"/>
-      <c r="F51" s="29"/>
-      <c r="G51" s="29"/>
-      <c r="H51" s="29"/>
+      <c r="A51" s="38"/>
+      <c r="B51" s="35"/>
+      <c r="C51" s="35"/>
+      <c r="D51" s="35"/>
+      <c r="E51" s="35"/>
+      <c r="F51" s="35"/>
+      <c r="G51" s="35"/>
+      <c r="H51" s="35"/>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
@@ -3307,14 +3991,14 @@
       <c r="K53" s="1"/>
     </row>
     <row r="54" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A54" s="32"/>
-      <c r="B54" s="29"/>
-      <c r="C54" s="29"/>
-      <c r="D54" s="29"/>
-      <c r="E54" s="29"/>
-      <c r="F54" s="29"/>
-      <c r="G54" s="29"/>
-      <c r="H54" s="29"/>
+      <c r="A54" s="38"/>
+      <c r="B54" s="35"/>
+      <c r="C54" s="35"/>
+      <c r="D54" s="35"/>
+      <c r="E54" s="35"/>
+      <c r="F54" s="35"/>
+      <c r="G54" s="35"/>
+      <c r="H54" s="35"/>
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
@@ -3333,14 +4017,14 @@
       <c r="K55" s="1"/>
     </row>
     <row r="56" spans="1:11" ht="20.25" customHeight="1">
-      <c r="A56" s="32"/>
-      <c r="B56" s="29"/>
-      <c r="C56" s="29"/>
-      <c r="D56" s="29"/>
-      <c r="E56" s="29"/>
-      <c r="F56" s="29"/>
-      <c r="G56" s="29"/>
-      <c r="H56" s="29"/>
+      <c r="A56" s="38"/>
+      <c r="B56" s="35"/>
+      <c r="C56" s="35"/>
+      <c r="D56" s="35"/>
+      <c r="E56" s="35"/>
+      <c r="F56" s="35"/>
+      <c r="G56" s="35"/>
+      <c r="H56" s="35"/>
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
@@ -3359,14 +4043,14 @@
       <c r="K57" s="1"/>
     </row>
     <row r="58" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A58" s="32"/>
-      <c r="B58" s="29"/>
-      <c r="C58" s="29"/>
-      <c r="D58" s="29"/>
-      <c r="E58" s="29"/>
-      <c r="F58" s="29"/>
-      <c r="G58" s="29"/>
-      <c r="H58" s="29"/>
+      <c r="A58" s="38"/>
+      <c r="B58" s="35"/>
+      <c r="C58" s="35"/>
+      <c r="D58" s="35"/>
+      <c r="E58" s="35"/>
+      <c r="F58" s="35"/>
+      <c r="G58" s="35"/>
+      <c r="H58" s="35"/>
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
@@ -3411,14 +4095,14 @@
       <c r="K61" s="1"/>
     </row>
     <row r="62" spans="1:11" ht="18" customHeight="1">
-      <c r="A62" s="32"/>
-      <c r="B62" s="29"/>
-      <c r="C62" s="29"/>
-      <c r="D62" s="29"/>
-      <c r="E62" s="29"/>
-      <c r="F62" s="29"/>
-      <c r="G62" s="29"/>
-      <c r="H62" s="29"/>
+      <c r="A62" s="38"/>
+      <c r="B62" s="35"/>
+      <c r="C62" s="35"/>
+      <c r="D62" s="35"/>
+      <c r="E62" s="35"/>
+      <c r="F62" s="35"/>
+      <c r="G62" s="35"/>
+      <c r="H62" s="35"/>
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
@@ -3450,14 +4134,14 @@
       <c r="K64" s="1"/>
     </row>
     <row r="65" spans="1:11" ht="19.5" customHeight="1">
-      <c r="A65" s="32"/>
-      <c r="B65" s="29"/>
-      <c r="C65" s="29"/>
-      <c r="D65" s="29"/>
-      <c r="E65" s="29"/>
-      <c r="F65" s="29"/>
-      <c r="G65" s="29"/>
-      <c r="H65" s="29"/>
+      <c r="A65" s="38"/>
+      <c r="B65" s="35"/>
+      <c r="C65" s="35"/>
+      <c r="D65" s="35"/>
+      <c r="E65" s="35"/>
+      <c r="F65" s="35"/>
+      <c r="G65" s="35"/>
+      <c r="H65" s="35"/>
       <c r="I65" s="1"/>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
@@ -3489,14 +4173,14 @@
       <c r="K67" s="1"/>
     </row>
     <row r="68" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A68" s="32"/>
-      <c r="B68" s="29"/>
-      <c r="C68" s="29"/>
-      <c r="D68" s="29"/>
-      <c r="E68" s="29"/>
-      <c r="F68" s="29"/>
-      <c r="G68" s="29"/>
-      <c r="H68" s="29"/>
+      <c r="A68" s="38"/>
+      <c r="B68" s="35"/>
+      <c r="C68" s="35"/>
+      <c r="D68" s="35"/>
+      <c r="E68" s="35"/>
+      <c r="F68" s="35"/>
+      <c r="G68" s="35"/>
+      <c r="H68" s="35"/>
       <c r="I68" s="1"/>
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
@@ -3587,12 +4271,13 @@
     <row r="80" spans="1:11" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="A68:H68"/>
+    <mergeCell ref="A51:H51"/>
+    <mergeCell ref="A54:H54"/>
+    <mergeCell ref="A56:H56"/>
+    <mergeCell ref="A58:H58"/>
+    <mergeCell ref="A62:H62"/>
+    <mergeCell ref="A65:H65"/>
     <mergeCell ref="A47:H47"/>
     <mergeCell ref="A17:H17"/>
     <mergeCell ref="A20:H20"/>
@@ -3605,13 +4290,12 @@
     <mergeCell ref="A37:H37"/>
     <mergeCell ref="A40:H40"/>
     <mergeCell ref="A43:H43"/>
-    <mergeCell ref="A68:H68"/>
-    <mergeCell ref="A51:H51"/>
-    <mergeCell ref="A54:H54"/>
-    <mergeCell ref="A56:H56"/>
-    <mergeCell ref="A58:H58"/>
-    <mergeCell ref="A62:H62"/>
-    <mergeCell ref="A65:H65"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A13:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>